<commit_message>
nterval data for exp
</commit_message>
<xml_diff>
--- a/ExpCurvFitting/ExpCurvFitting.Web/wwwroot/data_templates/data_template_poly.xlsx
+++ b/ExpCurvFitting/ExpCurvFitting.Web/wwwroot/data_templates/data_template_poly.xlsx
@@ -446,7 +446,7 @@
         <v>-1.5</v>
       </c>
       <c r="B2" s="4">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C2" s="4">
         <v>2.25</v>
@@ -460,7 +460,7 @@
         <v>0.5</v>
       </c>
       <c r="B3" s="4">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C3" s="4">
         <v>2.25</v>
@@ -474,7 +474,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="4">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C4" s="4">
         <v>3.5</v>
@@ -488,7 +488,7 @@
         <v>2.5</v>
       </c>
       <c r="B5" s="4">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C5" s="4">
         <v>10.25</v>
@@ -502,7 +502,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="4">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>4</v>
@@ -516,7 +516,7 @@
         <v>3.5</v>
       </c>
       <c r="B7" s="4">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C7" s="4">
         <v>17.25</v>

</xml_diff>